<commit_message>
Add multiple parsing job files
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="128">
   <si>
     <t>NAME</t>
   </si>
@@ -393,6 +393,9 @@
   </si>
   <si>
     <t>31=31+ SECS. WAITING</t>
+  </si>
+  <si>
+    <t>learningJob2</t>
   </si>
 </sst>
 </file>
@@ -981,6 +984,275 @@
         <v>126</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" t="s">
+        <v>104</v>
+      </c>
+      <c r="U3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V3" t="s">
+        <v>106</v>
+      </c>
+      <c r="W3" t="s">
+        <v>104</v>
+      </c>
+      <c r="X3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>114</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>115</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>119</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>120</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>95</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>93</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>123</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>124</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>125</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add feature for Dictionary
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -563,13 +563,13 @@
     <t>93</t>
   </si>
   <si>
-    <t>E</t>
+    <t>Expert Calling Ratio</t>
   </si>
   <si>
     <t>70</t>
   </si>
   <si>
-    <t>W40</t>
+    <t>Agent WorkTime = 40</t>
   </si>
   <si>
     <t>100</t>

</xml_diff>